<commit_message>
Functional version for Visual Basic Consumer
</commit_message>
<xml_diff>
--- a/C#Models/Consumer/Data.xlsx
+++ b/C#Models/Consumer/Data.xlsx
@@ -1,58 +1,93 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="80" yWindow="70" windowWidth="28700" windowHeight="12300"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="124519"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <x:bookViews>
+    <x:workbookView xWindow="80" yWindow="70" windowWidth="28700" windowHeight="12300" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="124519"/>
+</x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <x:si>
+    <x:t>vendor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>invoiceNumber</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bank Account: 7387324</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INVOICE # 850888</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-</styleSheet>
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -339,13 +374,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A1" sqref="A1 A1:B2"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.5"/>
+  <x:cols>
+    <x:col min="1" max="1" width="16.726562" style="2" customWidth="1"/>
+    <x:col min="2" max="2" width="17.632812" style="2" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:2">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2">
+      <x:c r="A2" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Added invoice template and improved producer and consumer.
</commit_message>
<xml_diff>
--- a/C#Models/Consumer/Data.xlsx
+++ b/C#Models/Consumer/Data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
   <x:bookViews>
-    <x:workbookView xWindow="80" yWindow="70" windowWidth="28700" windowHeight="12300" firstSheet="0" activeTab="0"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="124519"/>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <x:si>
     <x:t>vendor</x:t>
   </x:si>
@@ -23,10 +22,16 @@
     <x:t>invoiceNumber</x:t>
   </x:si>
   <x:si>
-    <x:t>Bank Account: 7387324</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INVOICE # 850888</x:t>
+    <x:t>MINDSHERPA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>85420</x:t>
+  </x:si>
+  <x:si>
+    <x:t>851244</x:t>
+  </x:si>
+  <x:si>
+    <x:t>850888</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -36,14 +41,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="2">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
+  <x:fonts count="1">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -61,23 +59,30 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  <x:cellXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -86,11 +91,10 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </x:styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -373,50 +377,52 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B1"/>
+  <x:dimension ref="A1:B4"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A1" sqref="A1 A1:B2"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.5"/>
-  <x:cols>
-    <x:col min="1" max="1" width="16.726562" style="2" customWidth="1"/>
-    <x:col min="2" max="2" width="17.632812" style="2" customWidth="1"/>
-  </x:cols>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:2">
-      <x:c r="A1" s="2" t="s">
+      <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
+      <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2">
-      <x:c r="A2" s="2" t="s">
+      <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B2" s="2" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
-      <x:c r="A3" s="2" t="s">
+      <x:c r="A3" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B3" s="2" t="s">
-        <x:v>3</x:v>
+      <x:c r="B3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>

</xml_diff>